<commit_message>
adding survey ID filter (slope fix)
</commit_message>
<xml_diff>
--- a/Cod_snowcrab_through2024_crab_ESP.xlsx
+++ b/Cod_snowcrab_through2024_crab_ESP.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20412"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kerim.aydin\Work\src\reem_diets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B09E23E3-C200-4671-B009-9BCC1F88974E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C9FC73-1F51-484C-AC35-480C3E615AA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9900"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cod_snowcrab_through2024_crab_E" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1659,50 +1659,6 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>478155</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>279837</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>115714</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FB63838-916E-4AF7-AB22-3F7F3DA78DFC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2916555" y="1685925"/>
-          <a:ext cx="6507282" cy="3135139"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2004,21 +1960,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1985</v>
       </c>
@@ -2026,7 +1982,7 @@
         <v>1469.98433</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1986</v>
       </c>
@@ -2034,7 +1990,7 @@
         <v>1047.4596120000001</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1987</v>
       </c>
@@ -2042,7 +1998,7 @@
         <v>1478.694487</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1988</v>
       </c>
@@ -2050,7 +2006,7 @@
         <v>568.57825009999999</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1989</v>
       </c>
@@ -2058,7 +2014,7 @@
         <v>1086.195119</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1990</v>
       </c>
@@ -2066,7 +2022,7 @@
         <v>778.97374400000001</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1991</v>
       </c>
@@ -2074,7 +2030,7 @@
         <v>834.18780140000001</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1992</v>
       </c>
@@ -2082,7 +2038,7 @@
         <v>415.22017249999999</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1993</v>
       </c>
@@ -2090,7 +2046,7 @@
         <v>510.15002299999998</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1994</v>
       </c>
@@ -2098,7 +2054,7 @@
         <v>1180.12318</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1995</v>
       </c>
@@ -2106,7 +2062,7 @@
         <v>961.26825229999997</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1996</v>
       </c>
@@ -2114,7 +2070,7 @@
         <v>1006.150806</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1997</v>
       </c>
@@ -2122,7 +2078,7 @@
         <v>969.49657009999999</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1998</v>
       </c>
@@ -2130,7 +2086,7 @@
         <v>636.52645870000003</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1999</v>
       </c>
@@ -2138,7 +2094,7 @@
         <v>590.87502870000003</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2000</v>
       </c>
@@ -2146,7 +2102,7 @@
         <v>838.01948189999996</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2001</v>
       </c>
@@ -2154,7 +2110,7 @@
         <v>1029.9061750000001</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2002</v>
       </c>
@@ -2162,7 +2118,7 @@
         <v>628.42804349999994</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2003</v>
       </c>
@@ -2170,7 +2126,7 @@
         <v>569.42104040000004</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2004</v>
       </c>
@@ -2178,7 +2134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2005</v>
       </c>
@@ -2186,7 +2142,7 @@
         <v>757.76309590000005</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2006</v>
       </c>
@@ -2194,7 +2150,7 @@
         <v>587.6786085</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2007</v>
       </c>
@@ -2202,7 +2158,7 @@
         <v>460.5743008</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2008</v>
       </c>
@@ -2210,7 +2166,7 @@
         <v>811.44901930000003</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2009</v>
       </c>
@@ -2218,7 +2174,7 @@
         <v>457.19864589999997</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2010</v>
       </c>
@@ -2226,7 +2182,7 @@
         <v>536.06783740000003</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2011</v>
       </c>
@@ -2234,7 +2190,7 @@
         <v>765.79463769999995</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2012</v>
       </c>
@@ -2242,7 +2198,7 @@
         <v>591.99830529999997</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2013</v>
       </c>
@@ -2250,7 +2206,7 @@
         <v>881.01376389999996</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2014</v>
       </c>
@@ -2258,7 +2214,7 @@
         <v>1619.8550299999999</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2015</v>
       </c>
@@ -2266,7 +2222,7 @@
         <v>2274.7604660000002</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2016</v>
       </c>
@@ -2274,7 +2230,7 @@
         <v>2461.7726699999998</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2017</v>
       </c>
@@ -2282,7 +2238,7 @@
         <v>882.78815580000003</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2018</v>
       </c>
@@ -2290,7 +2246,7 @@
         <v>1271.157933</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2019</v>
       </c>
@@ -2298,7 +2254,7 @@
         <v>847.17344370000001</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2020</v>
       </c>
@@ -2306,7 +2262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2021</v>
       </c>
@@ -2314,7 +2270,7 @@
         <v>847.36275869999997</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2022</v>
       </c>
@@ -2322,7 +2278,7 @@
         <v>631.14978389999999</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2023</v>
       </c>
@@ -2330,7 +2286,7 @@
         <v>511.84274850000003</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2024</v>
       </c>

</xml_diff>